<commit_message>
fix: mbiles creation when properties are nested
</commit_message>
<xml_diff>
--- a/test/resources/datasets/dataset-extensions.xlsx
+++ b/test/resources/datasets/dataset-extensions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">label</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t xml:space="preserve">19 rue de la voie lactée saint avé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val d’oust</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
@@ -52,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,13 +140,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.25"/>
@@ -169,6 +176,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>